<commit_message>
generated SJL schedules data
</commit_message>
<xml_diff>
--- a/data/horarios/horarios.sjl.raw.xlsx
+++ b/data/horarios/horarios.sjl.raw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dev\Documents\GitHub\fcc-pregrado-horarios-y-matriculas-xlsx-to-json\data\horarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C4BA08E-FC43-495B-8B74-2BD710990F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A6AA8B1D-7503-4774-BD35-F3E9B571F914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{A590CD18-6595-4A21-B343-4364D8886C09}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D79CC4F6-7FBB-4B7C-AA03-0EB67C4CD318}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -93,13 +93,124 @@
     <t>SÁBADO</t>
   </si>
   <si>
+    <t>GT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HISTORIA DEL PERÚ EN EL CONTEXTO MUNDIAL CONTEMPORÁNEO </t>
+  </si>
+  <si>
+    <t>SJL 72-T</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>CAYUELA BARRUEZO, MIGUEL ÁNGEL</t>
+  </si>
+  <si>
+    <t>14:00 -15:30 /15:30 - 17:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MATEMÁTICA I </t>
+  </si>
+  <si>
+    <t>CHUQUISPUMA CAYCHO, MIGUEL LUIS</t>
+  </si>
+  <si>
+    <t>14:00-15:30 / 15:30-17:00 / 17:00-17:45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FILOSOFÍA Y ÉTICA </t>
+  </si>
+  <si>
+    <t>FERRADAS MARTINEZ, MÓNICA DE LOURDES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11:00-14:00 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESARROLLO PERSONAL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">QUESQUÉN ALARCÓN, ERICK </t>
+  </si>
+  <si>
+    <t>14:30-16:00 / 16:00-17:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LENGUAJE I </t>
+  </si>
+  <si>
+    <t>RONCEROS LEVANO ALIDE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MÉTODOS DE ESTUDIO UNIVERSITARIO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:00-15:30 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 17:00-18:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOCTRINA CONTABLE </t>
+  </si>
+  <si>
+    <t>SALAZAR VARGAS, MONICA BETSABE</t>
+  </si>
+  <si>
+    <t>15:30-17:00 / 17:00-18:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INGLÉS I </t>
+  </si>
+  <si>
+    <t>ZUTA ZUMAETA, FRANCISCO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15:30-17:00 / 17:00-18:30 </t>
+  </si>
+  <si>
+    <t>AUD</t>
+  </si>
+  <si>
+    <t>SJL 73-T</t>
+  </si>
+  <si>
+    <t>14:00-15:30 / 15:30-17:00</t>
+  </si>
+  <si>
+    <t>MARCELO MALLQUI, MARCO ANTONIO</t>
+  </si>
+  <si>
+    <t>17:00-18:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17:00-18:30 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">OBREGÓN NICOLAS, KARIM GRACE </t>
+  </si>
+  <si>
+    <t>QUISPE SANCHEZ, NORMA</t>
+  </si>
+  <si>
+    <t>ROMERO LARRREATEGUI, EDWARD FREDERIk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15:30-17:00 </t>
+  </si>
+  <si>
+    <t>14:00-15:30 / 17:00-18:30</t>
+  </si>
+  <si>
     <t>C</t>
   </si>
   <si>
     <t>ESTADÍSTICA DESCRIPTIVA Y PROBABILIDADES</t>
   </si>
   <si>
-    <t>SJL 01-M</t>
+    <t>SJL 71-M</t>
   </si>
   <si>
     <t>M</t>
@@ -123,9 +234,6 @@
     <t>ECONOMÍA GENERAL</t>
   </si>
   <si>
-    <t>MARCELO MALLQUI, MARCO ANTONIO</t>
-  </si>
-  <si>
     <t>08:00-09:30 / 09:40-11:10</t>
   </si>
   <si>
@@ -153,16 +261,7 @@
     <t>DERECHO TRIBUTARIO</t>
   </si>
   <si>
-    <t xml:space="preserve">HISTORIA DEL PERÚ EN EL CONTEXTO MUNDIAL CONTEMPORÁNEO </t>
-  </si>
-  <si>
-    <t>SJL 01-T</t>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>CAYUELA BARRUEZO, MIGUEL ÁNGEL</t>
+    <t>SJL 71-T</t>
   </si>
   <si>
     <t>09:40-11:10</t>
@@ -171,118 +270,19 @@
     <t>15:30 -17:00 / 17.00 - 18:30</t>
   </si>
   <si>
-    <t xml:space="preserve">MÉTODOS DE ESTUDIO UNIVERSITARIO </t>
-  </si>
-  <si>
     <t>CHUMBE RODRÍGUEZ, ALDO CHRISTIAN</t>
   </si>
   <si>
     <t>15:30-17:00/ 17:00-18:30</t>
   </si>
   <si>
-    <t xml:space="preserve">MATEMÁTICA I </t>
-  </si>
-  <si>
-    <t>CHUQUISPUMA CAYCHO, MIGUEL LUIS</t>
-  </si>
-  <si>
-    <t>14:00-15:30 / 15:30-17:00 / 17:00-17:45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LENGUAJE I </t>
-  </si>
-  <si>
     <t>PUMA HANCCO, MELISSA JENNIFER</t>
   </si>
   <si>
-    <t xml:space="preserve">DESARROLLO PERSONAL </t>
-  </si>
-  <si>
-    <t>QUISPE SANCHEZ, NORMA</t>
-  </si>
-  <si>
-    <t>14:00-15:30 / 15:30-17:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FILOSOFÍA Y ÉTICA </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 15:30-17:00 / 17:00-18:30</t>
   </si>
   <si>
-    <t xml:space="preserve">DOCTRINA CONTABLE </t>
-  </si>
-  <si>
-    <t>SALAZAR VARGAS, MONICA BETSABE</t>
-  </si>
-  <si>
     <t>14:00-15:30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INGLÉS I </t>
-  </si>
-  <si>
-    <t>ZUTA ZUMAETA, FRANCISCO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14:00-15:30 </t>
-  </si>
-  <si>
-    <t>17:00-18:30</t>
-  </si>
-  <si>
-    <t>GT</t>
-  </si>
-  <si>
-    <t>SJL 02-T</t>
-  </si>
-  <si>
-    <t>14:00 -15:30 /15:30 - 17:00</t>
-  </si>
-  <si>
-    <t>FERRADAS MARTINEZ, MÓNICA DE LOURDES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11:00-14:00 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">QUESQUÉN ALARCÓN, ERICK </t>
-  </si>
-  <si>
-    <t>14:30-16:00 / 16:00-17:30</t>
-  </si>
-  <si>
-    <t>RONCEROS LEVANO ALIDE</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 17:00-18:30</t>
-  </si>
-  <si>
-    <t>15:30-17:00 / 17:00-18:30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15:30-17:00 / 17:00-18:30 </t>
-  </si>
-  <si>
-    <t>AUD</t>
-  </si>
-  <si>
-    <t>SJL 03-T</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17:00-18:30 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">OBREGÓN NICOLAS, KARIM GRACE </t>
-  </si>
-  <si>
-    <t>ROMERO LARRREATEGUI, EDWARD FREDERIk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15:30-17:00 </t>
-  </si>
-  <si>
-    <t>14:00-15:30 / 17:00-18:30</t>
   </si>
 </sst>
 </file>
@@ -335,6 +335,33 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{909D560A-39D7-4756-AA76-4FD509BB71BA}" name="Table1" displayName="Table1" ref="A1:R32" totalsRowShown="0">
+  <autoFilter ref="A1:R32" xr:uid="{909D560A-39D7-4756-AA76-4FD509BB71BA}"/>
+  <tableColumns count="18">
+    <tableColumn id="1" xr3:uid="{B9084FB0-200A-4782-B295-3976131443BB}" name="PLAN DE_x000a_ESTUDIOS"/>
+    <tableColumn id="2" xr3:uid="{12A9F28C-7415-48D9-A30B-1CCF47DE550E}" name="CICLO"/>
+    <tableColumn id="3" xr3:uid="{5AE0FF9F-DEA6-48B8-BB67-E2BC6E36B0D4}" name="EP"/>
+    <tableColumn id="4" xr3:uid="{5AFBACF5-3A43-4797-8A56-5F1D089E3F3C}" name="CÓD."/>
+    <tableColumn id="5" xr3:uid="{7831B018-75C7-40FF-BEF0-A5CEF86D17D1}" name="ASIGNATURAS"/>
+    <tableColumn id="6" xr3:uid="{CB49C88C-4866-44DB-8394-89FE4AA0CC77}" name="H.SEM"/>
+    <tableColumn id="7" xr3:uid="{25F74BDF-80B5-49F2-96A4-0146DCC7287D}" name="HT"/>
+    <tableColumn id="8" xr3:uid="{DF80AEAB-800B-45A9-8A02-4A9663345CDC}" name="HP"/>
+    <tableColumn id="9" xr3:uid="{5AD94F9B-CD65-4BA7-805B-024A71EA63D4}" name="CRED."/>
+    <tableColumn id="10" xr3:uid="{F4706053-ACAE-45BE-9FC8-CF9661B3CD45}" name="AULA"/>
+    <tableColumn id="11" xr3:uid="{30C8D27D-483D-47B4-B068-B5277F1FBE20}" name="TURNO"/>
+    <tableColumn id="12" xr3:uid="{17BE0E1A-CD4C-42FB-86E6-FFBFB8D43D89}" name="DOCENTE"/>
+    <tableColumn id="13" xr3:uid="{C25FBEFA-D2E4-4F49-A4AE-61439797D91E}" name="LUNES"/>
+    <tableColumn id="14" xr3:uid="{BCE17836-5D88-4C29-AADF-669843E4F735}" name="MARTES"/>
+    <tableColumn id="15" xr3:uid="{7CF8AA23-E44B-403E-AE1F-0439BA194046}" name="MIÉRCOLES"/>
+    <tableColumn id="16" xr3:uid="{90BD880F-ED0D-4CE2-B488-A78CED9B40A7}" name="JUEVES"/>
+    <tableColumn id="17" xr3:uid="{88E89921-FF5D-4E64-A1F1-EB658B4A75CC}" name="VIERNES"/>
+    <tableColumn id="18" xr3:uid="{5871AF96-3207-4BE2-AB79-B23B9DB43426}" name="SÁBADO"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -653,26 +680,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6E2E917-33BD-4D10-A88F-B35A9E473D8B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47AD2462-FA73-4617-836D-7834D2E54DA3}">
   <dimension ref="A1:R32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection sqref="A1:R32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" customWidth="1"/>
     <col min="5" max="5" width="60.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" customWidth="1"/>
+    <col min="7" max="7" width="5.42578125" customWidth="1"/>
+    <col min="8" max="8" width="5.5703125" customWidth="1"/>
+    <col min="9" max="9" width="8.28515625" customWidth="1"/>
     <col min="10" max="10" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" customWidth="1"/>
     <col min="12" max="12" width="40" bestFit="1" customWidth="1"/>
     <col min="13" max="18" width="34.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -738,13 +765,13 @@
         <v>2022</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
       </c>
       <c r="D2">
-        <v>111351</v>
+        <v>112145</v>
       </c>
       <c r="E2" t="s">
         <v>19</v>
@@ -770,7 +797,7 @@
       <c r="L2" t="s">
         <v>22</v>
       </c>
-      <c r="P2" t="s">
+      <c r="O2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -779,28 +806,28 @@
         <v>2022</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
       </c>
       <c r="D3">
-        <v>111349</v>
+        <v>112146</v>
       </c>
       <c r="E3" t="s">
         <v>24</v>
       </c>
       <c r="F3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H3">
         <v>4</v>
       </c>
       <c r="I3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J3" t="s">
         <v>20</v>
@@ -820,13 +847,13 @@
         <v>2022</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
         <v>18</v>
       </c>
       <c r="D4">
-        <v>111352</v>
+        <v>112144</v>
       </c>
       <c r="E4" t="s">
         <v>27</v>
@@ -861,28 +888,28 @@
         <v>2022</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
       </c>
       <c r="D5">
-        <v>111350</v>
+        <v>112149</v>
       </c>
       <c r="E5" t="s">
         <v>30</v>
       </c>
       <c r="F5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G5">
         <v>2</v>
       </c>
       <c r="H5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J5" t="s">
         <v>20</v>
@@ -891,10 +918,10 @@
         <v>21</v>
       </c>
       <c r="L5" t="s">
-        <v>28</v>
-      </c>
-      <c r="O5" t="s">
         <v>31</v>
+      </c>
+      <c r="R5" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -902,25 +929,25 @@
         <v>2022</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
         <v>18</v>
       </c>
       <c r="D6">
-        <v>111353</v>
+        <v>112142</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I6">
         <v>3</v>
@@ -932,10 +959,10 @@
         <v>21</v>
       </c>
       <c r="L6" t="s">
-        <v>33</v>
-      </c>
-      <c r="M6" t="s">
-        <v>29</v>
+        <v>34</v>
+      </c>
+      <c r="N6" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -943,16 +970,16 @@
         <v>2022</v>
       </c>
       <c r="B7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C7" t="s">
         <v>18</v>
       </c>
       <c r="D7">
-        <v>111354</v>
+        <v>112143</v>
       </c>
       <c r="E7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F7">
         <v>4</v>
@@ -973,13 +1000,13 @@
         <v>21</v>
       </c>
       <c r="L7" t="s">
-        <v>33</v>
-      </c>
-      <c r="N7" t="s">
-        <v>35</v>
-      </c>
-      <c r="P7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M7" t="s">
         <v>36</v>
+      </c>
+      <c r="O7" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -987,16 +1014,16 @@
         <v>2022</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
       </c>
       <c r="D8">
-        <v>111355</v>
+        <v>112147</v>
       </c>
       <c r="E8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F8">
         <v>4</v>
@@ -1017,10 +1044,10 @@
         <v>21</v>
       </c>
       <c r="L8" t="s">
-        <v>33</v>
-      </c>
-      <c r="N8" t="s">
-        <v>29</v>
+        <v>39</v>
+      </c>
+      <c r="P8" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -1034,10 +1061,10 @@
         <v>18</v>
       </c>
       <c r="D9">
-        <v>111145</v>
+        <v>112148</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F9">
         <v>4</v>
@@ -1052,18 +1079,15 @@
         <v>3</v>
       </c>
       <c r="J9" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="K9" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="L9" t="s">
-        <v>41</v>
-      </c>
-      <c r="N9" t="s">
         <v>42</v>
       </c>
-      <c r="P9" t="s">
+      <c r="M9" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1075,13 +1099,13 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="D10">
-        <v>111143</v>
+        <v>113145</v>
       </c>
       <c r="E10" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="F10">
         <v>4</v>
@@ -1096,16 +1120,16 @@
         <v>3</v>
       </c>
       <c r="J10" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="K10" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="L10" t="s">
-        <v>45</v>
-      </c>
-      <c r="N10" t="s">
-        <v>46</v>
+        <v>22</v>
+      </c>
+      <c r="M10" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -1116,37 +1140,37 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="D11">
-        <v>111146</v>
+        <v>113144</v>
       </c>
       <c r="E11" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="F11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H11">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I11">
         <v>3</v>
       </c>
       <c r="J11" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="K11" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="L11" t="s">
-        <v>48</v>
-      </c>
-      <c r="O11" t="s">
-        <v>49</v>
+        <v>28</v>
+      </c>
+      <c r="N11" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -1157,36 +1181,39 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="D12">
-        <v>111142</v>
+        <v>113143</v>
       </c>
       <c r="E12" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="F12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H12">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I12">
         <v>3</v>
       </c>
       <c r="J12" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="K12" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="L12" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="M12" t="s">
+        <v>48</v>
+      </c>
+      <c r="O12" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1198,37 +1225,37 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="D13">
-        <v>111149</v>
+        <v>113142</v>
       </c>
       <c r="E13" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="F13">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I13">
         <v>3</v>
       </c>
       <c r="J13" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="K13" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="L13" t="s">
-        <v>53</v>
-      </c>
-      <c r="R13" t="s">
-        <v>54</v>
+        <v>50</v>
+      </c>
+      <c r="P13" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -1239,13 +1266,13 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="D14">
-        <v>111144</v>
+        <v>113149</v>
       </c>
       <c r="E14" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="F14">
         <v>4</v>
@@ -1260,16 +1287,16 @@
         <v>3</v>
       </c>
       <c r="J14" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="K14" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="L14" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>56</v>
+        <v>51</v>
+      </c>
+      <c r="O14" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -1280,40 +1307,37 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="D15">
-        <v>111147</v>
+        <v>113146</v>
       </c>
       <c r="E15" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="F15">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H15">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I15">
         <v>3</v>
       </c>
       <c r="J15" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="K15" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="L15" t="s">
-        <v>58</v>
-      </c>
-      <c r="N15" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>59</v>
+        <v>52</v>
+      </c>
+      <c r="R15" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -1324,13 +1348,13 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="D16">
-        <v>111148</v>
+        <v>113147</v>
       </c>
       <c r="E16" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="F16">
         <v>4</v>
@@ -1345,19 +1369,19 @@
         <v>3</v>
       </c>
       <c r="J16" t="s">
+        <v>45</v>
+      </c>
+      <c r="K16" t="s">
+        <v>21</v>
+      </c>
+      <c r="L16" t="s">
         <v>39</v>
       </c>
-      <c r="K16" t="s">
-        <v>40</v>
-      </c>
-      <c r="L16" t="s">
-        <v>61</v>
-      </c>
-      <c r="P16" t="s">
-        <v>62</v>
-      </c>
-      <c r="R16" t="s">
-        <v>63</v>
+      <c r="N16" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
@@ -1368,13 +1392,13 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="D17">
-        <v>112145</v>
+        <v>113148</v>
       </c>
       <c r="E17" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F17">
         <v>4</v>
@@ -1389,16 +1413,16 @@
         <v>3</v>
       </c>
       <c r="J17" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="K17" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="L17" t="s">
-        <v>41</v>
-      </c>
-      <c r="O17" t="s">
-        <v>66</v>
+        <v>42</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
@@ -1406,40 +1430,40 @@
         <v>2022</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D18">
-        <v>112146</v>
+        <v>111351</v>
       </c>
       <c r="E18" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="F18">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I18">
         <v>3</v>
       </c>
       <c r="J18" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="K18" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="L18" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>49</v>
+        <v>59</v>
+      </c>
+      <c r="P18" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
@@ -1447,40 +1471,40 @@
         <v>2022</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D19">
-        <v>112144</v>
+        <v>111349</v>
       </c>
       <c r="E19" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="F19">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G19">
         <v>2</v>
       </c>
       <c r="H19">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I19">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J19" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="K19" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="L19" t="s">
-        <v>67</v>
-      </c>
-      <c r="R19" t="s">
-        <v>68</v>
+        <v>62</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
@@ -1488,17 +1512,17 @@
         <v>2022</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C20" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20">
+        <v>111352</v>
+      </c>
+      <c r="E20" t="s">
         <v>64</v>
       </c>
-      <c r="D20">
-        <v>112149</v>
-      </c>
-      <c r="E20" t="s">
-        <v>52</v>
-      </c>
       <c r="F20">
         <v>4</v>
       </c>
@@ -1512,16 +1536,16 @@
         <v>3</v>
       </c>
       <c r="J20" t="s">
+        <v>57</v>
+      </c>
+      <c r="K20" t="s">
+        <v>58</v>
+      </c>
+      <c r="L20" t="s">
+        <v>47</v>
+      </c>
+      <c r="R20" t="s">
         <v>65</v>
-      </c>
-      <c r="K20" t="s">
-        <v>40</v>
-      </c>
-      <c r="L20" t="s">
-        <v>69</v>
-      </c>
-      <c r="R20" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
@@ -1529,40 +1553,40 @@
         <v>2022</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D21">
-        <v>112142</v>
+        <v>111350</v>
       </c>
       <c r="E21" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="F21">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H21">
         <v>4</v>
       </c>
       <c r="I21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J21" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="K21" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="L21" t="s">
-        <v>71</v>
-      </c>
-      <c r="N21" t="s">
-        <v>49</v>
+        <v>47</v>
+      </c>
+      <c r="O21" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
@@ -1570,16 +1594,16 @@
         <v>2022</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D22">
-        <v>112143</v>
+        <v>111353</v>
       </c>
       <c r="E22" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="F22">
         <v>4</v>
@@ -1594,19 +1618,16 @@
         <v>3</v>
       </c>
       <c r="J22" t="s">
+        <v>57</v>
+      </c>
+      <c r="K22" t="s">
+        <v>58</v>
+      </c>
+      <c r="L22" t="s">
+        <v>69</v>
+      </c>
+      <c r="M22" t="s">
         <v>65</v>
-      </c>
-      <c r="K22" t="s">
-        <v>40</v>
-      </c>
-      <c r="L22" t="s">
-        <v>71</v>
-      </c>
-      <c r="M22" t="s">
-        <v>62</v>
-      </c>
-      <c r="O22" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
@@ -1614,40 +1635,43 @@
         <v>2022</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D23">
-        <v>112147</v>
+        <v>111354</v>
       </c>
       <c r="E23" t="s">
+        <v>70</v>
+      </c>
+      <c r="F23">
+        <v>4</v>
+      </c>
+      <c r="G23">
+        <v>2</v>
+      </c>
+      <c r="H23">
+        <v>2</v>
+      </c>
+      <c r="I23">
+        <v>3</v>
+      </c>
+      <c r="J23" t="s">
         <v>57</v>
       </c>
-      <c r="F23">
-        <v>4</v>
-      </c>
-      <c r="G23">
-        <v>2</v>
-      </c>
-      <c r="H23">
-        <v>2</v>
-      </c>
-      <c r="I23">
-        <v>3</v>
-      </c>
-      <c r="J23" t="s">
-        <v>65</v>
-      </c>
       <c r="K23" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="L23" t="s">
-        <v>58</v>
+        <v>69</v>
+      </c>
+      <c r="N23" t="s">
+        <v>71</v>
       </c>
       <c r="P23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
@@ -1655,16 +1679,16 @@
         <v>2022</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D24">
-        <v>112148</v>
+        <v>111355</v>
       </c>
       <c r="E24" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="F24">
         <v>4</v>
@@ -1679,16 +1703,16 @@
         <v>3</v>
       </c>
       <c r="J24" t="s">
+        <v>57</v>
+      </c>
+      <c r="K24" t="s">
+        <v>58</v>
+      </c>
+      <c r="L24" t="s">
+        <v>69</v>
+      </c>
+      <c r="N24" t="s">
         <v>65</v>
-      </c>
-      <c r="K24" t="s">
-        <v>40</v>
-      </c>
-      <c r="L24" t="s">
-        <v>61</v>
-      </c>
-      <c r="M24" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
@@ -1699,37 +1723,40 @@
         <v>1</v>
       </c>
       <c r="C25" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25">
+        <v>111145</v>
+      </c>
+      <c r="E25" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25">
+        <v>4</v>
+      </c>
+      <c r="G25">
+        <v>2</v>
+      </c>
+      <c r="H25">
+        <v>2</v>
+      </c>
+      <c r="I25">
+        <v>3</v>
+      </c>
+      <c r="J25" t="s">
+        <v>74</v>
+      </c>
+      <c r="K25" t="s">
+        <v>21</v>
+      </c>
+      <c r="L25" t="s">
+        <v>22</v>
+      </c>
+      <c r="N25" t="s">
         <v>75</v>
       </c>
-      <c r="D25">
-        <v>113145</v>
-      </c>
-      <c r="E25" t="s">
-        <v>38</v>
-      </c>
-      <c r="F25">
-        <v>4</v>
-      </c>
-      <c r="G25">
-        <v>2</v>
-      </c>
-      <c r="H25">
-        <v>2</v>
-      </c>
-      <c r="I25">
-        <v>3</v>
-      </c>
-      <c r="J25" t="s">
+      <c r="P25" t="s">
         <v>76</v>
-      </c>
-      <c r="K25" t="s">
-        <v>40</v>
-      </c>
-      <c r="L25" t="s">
-        <v>41</v>
-      </c>
-      <c r="M25" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
@@ -1740,13 +1767,13 @@
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="D26">
-        <v>113144</v>
+        <v>111143</v>
       </c>
       <c r="E26" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="F26">
         <v>4</v>
@@ -1761,16 +1788,16 @@
         <v>3</v>
       </c>
       <c r="J26" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K26" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="L26" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="N26" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
@@ -1781,40 +1808,37 @@
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="D27">
-        <v>113143</v>
+        <v>111146</v>
       </c>
       <c r="E27" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="F27">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H27">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I27">
         <v>3</v>
       </c>
       <c r="J27" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K27" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="L27" t="s">
-        <v>28</v>
-      </c>
-      <c r="M27" t="s">
-        <v>63</v>
+        <v>25</v>
       </c>
       <c r="O27" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
@@ -1825,13 +1849,13 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="D28">
-        <v>113142</v>
+        <v>111142</v>
       </c>
       <c r="E28" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="F28">
         <v>5</v>
@@ -1846,16 +1870,16 @@
         <v>3</v>
       </c>
       <c r="J28" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K28" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="L28" t="s">
-        <v>78</v>
-      </c>
-      <c r="P28" t="s">
-        <v>49</v>
+        <v>79</v>
+      </c>
+      <c r="M28" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
@@ -1866,13 +1890,13 @@
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="D29">
-        <v>113149</v>
+        <v>111144</v>
       </c>
       <c r="E29" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="F29">
         <v>4</v>
@@ -1887,16 +1911,16 @@
         <v>3</v>
       </c>
       <c r="J29" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K29" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="L29" t="s">
-        <v>53</v>
-      </c>
-      <c r="O29" t="s">
-        <v>54</v>
+        <v>51</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
@@ -1907,37 +1931,37 @@
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="D30">
-        <v>113146</v>
+        <v>111149</v>
       </c>
       <c r="E30" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="F30">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H30">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I30">
         <v>3</v>
       </c>
       <c r="J30" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K30" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="L30" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="R30" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
@@ -1948,13 +1972,13 @@
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="D31">
-        <v>113147</v>
+        <v>111147</v>
       </c>
       <c r="E31" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="F31">
         <v>4</v>
@@ -1969,19 +1993,19 @@
         <v>3</v>
       </c>
       <c r="J31" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K31" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="L31" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="N31" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="Q31" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
@@ -1992,13 +2016,13 @@
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="D32">
-        <v>113148</v>
+        <v>111148</v>
       </c>
       <c r="E32" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="F32">
         <v>4</v>
@@ -2013,19 +2037,25 @@
         <v>3</v>
       </c>
       <c r="J32" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K32" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="L32" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q32" t="s">
-        <v>81</v>
+        <v>42</v>
+      </c>
+      <c r="P32" t="s">
+        <v>36</v>
+      </c>
+      <c r="R32" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>